<commit_message>
Journal of Clinical & Translational Endocrinology flipped to open
</commit_message>
<xml_diff>
--- a/Bibsam_tidskriftslistor/scifree_data_elsevier.xlsx
+++ b/Bibsam_tidskriftslistor/scifree_data_elsevier.xlsx
@@ -20700,16 +20700,6 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -20725,6 +20715,16 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -20739,7 +20739,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G2290" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G2290" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:G2290"/>
   <sortState ref="A2:G2294">
     <sortCondition ref="A2:A2294"/>
@@ -21023,8 +21023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2200" workbookViewId="0">
-      <selection activeCell="D2239" sqref="D2239"/>
+    <sheetView tabSelected="1" topLeftCell="A1101" workbookViewId="0">
+      <selection activeCell="F1129" sqref="F1129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43594,7 +43594,7 @@
         <v>3018</v>
       </c>
       <c r="F1129" t="s">
-        <v>6699</v>
+        <v>0</v>
       </c>
       <c r="G1129" t="s">
         <v>6703</v>
@@ -66822,7 +66822,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>